<commit_message>
Design Phase 2025/09/16 - Updated ERD v3
</commit_message>
<xml_diff>
--- a/documentation/ERD.xlsx
+++ b/documentation/ERD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgalpo\Documents\BarangayManagementSystem\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADDC5C8-E297-4E4F-B5C2-EC9128B66CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846FFA63-A049-4BA2-B27F-E30C5B38BE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E5D6EDC0-E2F0-4D01-84F0-FC71D003CD96}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E5D6EDC0-E2F0-4D01-84F0-FC71D003CD96}"/>
   </bookViews>
   <sheets>
     <sheet name="ERD v1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6385" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6380" uniqueCount="479">
   <si>
     <t>auto_increment</t>
   </si>
@@ -1463,6 +1463,18 @@
   </si>
   <si>
     <t>phone_number</t>
+  </si>
+  <si>
+    <t>Deathdate</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>fk_Resident</t>
+  </si>
+  <si>
+    <t>fk_Association</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1621,6 +1633,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1636,13 +1654,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6351,72 +6362,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="88" name="Rectangle 87">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D591E2A-8051-4A4B-BE31-3564203BB1BB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="20478751" y="4457700"/>
-          <a:ext cx="7181850" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6748,13 +6693,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -14513,8 +14458,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91730</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -14532,12 +14477,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16573500" y="938213"/>
-          <a:ext cx="3905250" cy="3781425"/>
+          <a:off x="16590065" y="950637"/>
+          <a:ext cx="3909392" cy="3663397"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 87317"/>
+            <a:gd name="adj1" fmla="val 87500"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -14567,13 +14512,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>524291</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>168550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>2487</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>19464</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -21998,33 +21943,33 @@
       </c>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="G2" t="s">
         <v>353</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
       <c r="P2" t="s">
         <v>353</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
       <c r="Y2" t="s">
         <v>353</v>
       </c>
@@ -22364,13 +22309,13 @@
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
       <c r="K11" s="3" t="s">
         <v>40</v>
       </c>
@@ -22424,13 +22369,13 @@
       <c r="O12" s="3">
         <v>50</v>
       </c>
-      <c r="T12" s="12" t="s">
+      <c r="T12" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
       <c r="Y12" t="s">
         <v>353</v>
       </c>
@@ -22676,13 +22621,13 @@
       <c r="B19" t="s">
         <v>79</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="K19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="11"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="15"/>
       <c r="P19" t="s">
         <v>353</v>
       </c>
@@ -22703,13 +22648,13 @@
       </c>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
       <c r="G20" t="s">
         <v>353</v>
       </c>
@@ -22938,13 +22883,13 @@
       </c>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="T26" s="12" t="s">
+      <c r="T26" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="U26" s="12"/>
-      <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="12"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
       <c r="Y26" t="s">
         <v>353</v>
       </c>
@@ -22953,13 +22898,13 @@
       <c r="B27" t="s">
         <v>80</v>
       </c>
-      <c r="K27" s="9" t="s">
+      <c r="K27" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="11"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="15"/>
       <c r="P27" t="s">
         <v>353</v>
       </c>
@@ -22980,13 +22925,13 @@
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
       <c r="G28" t="s">
         <v>353</v>
       </c>
@@ -23250,35 +23195,35 @@
       <c r="B35" t="s">
         <v>81</v>
       </c>
-      <c r="T35" s="9" t="s">
+      <c r="T35" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
-      <c r="W35" s="10"/>
-      <c r="X35" s="11"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="15"/>
       <c r="Y35" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
       <c r="G36" t="s">
         <v>353</v>
       </c>
-      <c r="K36" s="9" t="s">
+      <c r="K36" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="11"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="15"/>
       <c r="P36" t="s">
         <v>353</v>
       </c>
@@ -23571,23 +23516,23 @@
       </c>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
       <c r="G44" t="s">
         <v>353</v>
       </c>
-      <c r="K44" s="9" t="s">
+      <c r="K44" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="11"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="15"/>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B45" s="2" t="s">
@@ -23655,13 +23600,13 @@
       <c r="O46" s="3">
         <v>10</v>
       </c>
-      <c r="T46" s="9" t="s">
+      <c r="T46" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="U46" s="10"/>
-      <c r="V46" s="10"/>
-      <c r="W46" s="10"/>
-      <c r="X46" s="11"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="15"/>
     </row>
     <row r="47" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B47" s="3" t="s">
@@ -23872,13 +23817,13 @@
       </c>
     </row>
     <row r="52" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
       <c r="G52" t="s">
         <v>353</v>
       </c>
@@ -24020,13 +23965,13 @@
       <c r="O56" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T56" s="9" t="s">
+      <c r="T56" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="U56" s="10"/>
-      <c r="V56" s="10"/>
-      <c r="W56" s="10"/>
-      <c r="X56" s="11"/>
+      <c r="U56" s="14"/>
+      <c r="V56" s="14"/>
+      <c r="W56" s="14"/>
+      <c r="X56" s="15"/>
       <c r="Y56" t="s">
         <v>353</v>
       </c>
@@ -24131,13 +24076,13 @@
       </c>
     </row>
     <row r="60" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
       <c r="G60" t="s">
         <v>353</v>
       </c>
@@ -24237,13 +24182,13 @@
       <c r="F63" s="3">
         <v>50</v>
       </c>
-      <c r="K63" s="9" t="s">
+      <c r="K63" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
-      <c r="N63" s="10"/>
-      <c r="O63" s="11"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="15"/>
       <c r="P63" t="s">
         <v>353</v>
       </c>
@@ -24343,13 +24288,13 @@
       <c r="O66" s="3">
         <v>10</v>
       </c>
-      <c r="T66" s="9" t="s">
+      <c r="T66" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="U66" s="10"/>
-      <c r="V66" s="10"/>
-      <c r="W66" s="10"/>
-      <c r="X66" s="11"/>
+      <c r="U66" s="14"/>
+      <c r="V66" s="14"/>
+      <c r="W66" s="14"/>
+      <c r="X66" s="15"/>
       <c r="Y66" t="s">
         <v>353</v>
       </c>
@@ -24390,13 +24335,13 @@
       </c>
     </row>
     <row r="68" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
       <c r="G68" t="s">
         <v>353</v>
       </c>
@@ -24675,13 +24620,13 @@
       <c r="B75" t="s">
         <v>101</v>
       </c>
-      <c r="K75" s="9" t="s">
+      <c r="K75" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="L75" s="10"/>
-      <c r="M75" s="10"/>
-      <c r="N75" s="10"/>
-      <c r="O75" s="11"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
+      <c r="N75" s="14"/>
+      <c r="O75" s="15"/>
       <c r="P75" t="s">
         <v>353</v>
       </c>
@@ -24702,13 +24647,13 @@
       </c>
     </row>
     <row r="76" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B76" s="12" t="s">
+      <c r="B76" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
       <c r="G76" t="s">
         <v>353</v>
       </c>
@@ -24885,13 +24830,13 @@
       <c r="O80" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T80" s="9" t="s">
+      <c r="T80" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="U80" s="10"/>
-      <c r="V80" s="10"/>
-      <c r="W80" s="10"/>
-      <c r="X80" s="11"/>
+      <c r="U80" s="14"/>
+      <c r="V80" s="14"/>
+      <c r="W80" s="14"/>
+      <c r="X80" s="15"/>
     </row>
     <row r="81" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B81" s="3" t="s">
@@ -24946,13 +24891,13 @@
       </c>
     </row>
     <row r="83" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="K83" s="9" t="s">
+      <c r="K83" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="L83" s="10"/>
-      <c r="M83" s="10"/>
-      <c r="N83" s="10"/>
-      <c r="O83" s="11"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
+      <c r="N83" s="14"/>
+      <c r="O83" s="15"/>
       <c r="P83" t="s">
         <v>353</v>
       </c>
@@ -24973,13 +24918,13 @@
       </c>
     </row>
     <row r="84" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B84" s="12" t="s">
+      <c r="B84" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
       <c r="G84" t="s">
         <v>353</v>
       </c>
@@ -25253,13 +25198,13 @@
       <c r="F90" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K90" s="9" t="s">
+      <c r="K90" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="L90" s="10"/>
-      <c r="M90" s="10"/>
-      <c r="N90" s="10"/>
-      <c r="O90" s="11"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="14"/>
+      <c r="N90" s="14"/>
+      <c r="O90" s="15"/>
       <c r="P90" t="s">
         <v>353</v>
       </c>
@@ -25300,25 +25245,25 @@
       <c r="O92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T92" s="9" t="s">
+      <c r="T92" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="U92" s="10"/>
-      <c r="V92" s="10"/>
-      <c r="W92" s="10"/>
-      <c r="X92" s="11"/>
+      <c r="U92" s="14"/>
+      <c r="V92" s="14"/>
+      <c r="W92" s="14"/>
+      <c r="X92" s="15"/>
       <c r="Y92" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="93" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="16"/>
+      <c r="E93" s="16"/>
+      <c r="F93" s="16"/>
       <c r="G93" t="s">
         <v>353</v>
       </c>
@@ -25663,13 +25608,13 @@
       <c r="O102" s="3">
         <v>50</v>
       </c>
-      <c r="T102" s="9" t="s">
+      <c r="T102" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="U102" s="10"/>
-      <c r="V102" s="10"/>
-      <c r="W102" s="10"/>
-      <c r="X102" s="11"/>
+      <c r="U102" s="14"/>
+      <c r="V102" s="14"/>
+      <c r="W102" s="14"/>
+      <c r="X102" s="15"/>
       <c r="Y102" t="s">
         <v>353</v>
       </c>
@@ -25903,13 +25848,13 @@
       <c r="B109" t="s">
         <v>113</v>
       </c>
-      <c r="K109" s="9" t="s">
+      <c r="K109" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="L109" s="10"/>
-      <c r="M109" s="10"/>
-      <c r="N109" s="10"/>
-      <c r="O109" s="11"/>
+      <c r="L109" s="14"/>
+      <c r="M109" s="14"/>
+      <c r="N109" s="14"/>
+      <c r="O109" s="15"/>
       <c r="T109" s="3" t="s">
         <v>11</v>
       </c>
@@ -26016,13 +25961,13 @@
       <c r="O112" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T112" s="9" t="s">
+      <c r="T112" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="U112" s="10"/>
-      <c r="V112" s="10"/>
-      <c r="W112" s="10"/>
-      <c r="X112" s="11"/>
+      <c r="U112" s="14"/>
+      <c r="V112" s="14"/>
+      <c r="W112" s="14"/>
+      <c r="X112" s="15"/>
       <c r="Y112" t="s">
         <v>353</v>
       </c>
@@ -26202,13 +26147,13 @@
       <c r="G118" t="s">
         <v>353</v>
       </c>
-      <c r="K118" s="9" t="s">
+      <c r="K118" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="L118" s="10"/>
-      <c r="M118" s="10"/>
-      <c r="N118" s="10"/>
-      <c r="O118" s="11"/>
+      <c r="L118" s="14"/>
+      <c r="M118" s="14"/>
+      <c r="N118" s="14"/>
+      <c r="O118" s="15"/>
       <c r="P118" t="s">
         <v>353</v>
       </c>
@@ -26453,13 +26398,13 @@
       <c r="F127" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K127" s="9" t="s">
+      <c r="K127" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="L127" s="10"/>
-      <c r="M127" s="10"/>
-      <c r="N127" s="10"/>
-      <c r="O127" s="11"/>
+      <c r="L127" s="14"/>
+      <c r="M127" s="14"/>
+      <c r="N127" s="14"/>
+      <c r="O127" s="15"/>
     </row>
     <row r="128" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B128" s="3" t="s">
@@ -26651,13 +26596,13 @@
       <c r="F136" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K136" s="9" t="s">
+      <c r="K136" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="L136" s="10"/>
-      <c r="M136" s="10"/>
-      <c r="N136" s="10"/>
-      <c r="O136" s="11"/>
+      <c r="L136" s="14"/>
+      <c r="M136" s="14"/>
+      <c r="N136" s="14"/>
+      <c r="O136" s="15"/>
     </row>
     <row r="137" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B137" s="3" t="s">
@@ -26793,13 +26738,13 @@
       <c r="B144" t="s">
         <v>151</v>
       </c>
-      <c r="K144" s="9" t="s">
+      <c r="K144" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="L144" s="10"/>
-      <c r="M144" s="10"/>
-      <c r="N144" s="10"/>
-      <c r="O144" s="11"/>
+      <c r="L144" s="14"/>
+      <c r="M144" s="14"/>
+      <c r="N144" s="14"/>
+      <c r="O144" s="15"/>
     </row>
     <row r="145" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B145" s="1" t="s">
@@ -26977,13 +26922,13 @@
       <c r="B152" t="s">
         <v>152</v>
       </c>
-      <c r="K152" s="9" t="s">
+      <c r="K152" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="L152" s="10"/>
-      <c r="M152" s="10"/>
-      <c r="N152" s="10"/>
-      <c r="O152" s="11"/>
+      <c r="L152" s="14"/>
+      <c r="M152" s="14"/>
+      <c r="N152" s="14"/>
+      <c r="O152" s="15"/>
     </row>
     <row r="153" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B153" s="4" t="s">
@@ -27161,13 +27106,13 @@
       <c r="B160" t="s">
         <v>153</v>
       </c>
-      <c r="K160" s="9" t="s">
+      <c r="K160" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L160" s="10"/>
-      <c r="M160" s="10"/>
-      <c r="N160" s="10"/>
-      <c r="O160" s="11"/>
+      <c r="L160" s="14"/>
+      <c r="M160" s="14"/>
+      <c r="N160" s="14"/>
+      <c r="O160" s="15"/>
     </row>
     <row r="161" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B161" s="4" t="s">
@@ -28851,19 +28796,18 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="K144:O144"/>
-    <mergeCell ref="K152:O152"/>
-    <mergeCell ref="K160:O160"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="K75:O75"/>
-    <mergeCell ref="K127:O127"/>
-    <mergeCell ref="K136:O136"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="K27:O27"/>
-    <mergeCell ref="K36:O36"/>
-    <mergeCell ref="K63:O63"/>
-    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="T56:X56"/>
+    <mergeCell ref="K109:O109"/>
+    <mergeCell ref="K118:O118"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="T92:X92"/>
+    <mergeCell ref="T102:X102"/>
+    <mergeCell ref="T112:X112"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="T66:X66"/>
+    <mergeCell ref="K90:O90"/>
+    <mergeCell ref="K83:O83"/>
+    <mergeCell ref="T80:X80"/>
     <mergeCell ref="T46:X46"/>
     <mergeCell ref="K19:O19"/>
     <mergeCell ref="B2:F2"/>
@@ -28878,18 +28822,19 @@
     <mergeCell ref="T26:X26"/>
     <mergeCell ref="T35:X35"/>
     <mergeCell ref="K44:O44"/>
-    <mergeCell ref="T56:X56"/>
-    <mergeCell ref="K109:O109"/>
-    <mergeCell ref="K118:O118"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="T92:X92"/>
-    <mergeCell ref="T102:X102"/>
-    <mergeCell ref="T112:X112"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="T66:X66"/>
-    <mergeCell ref="K90:O90"/>
-    <mergeCell ref="K83:O83"/>
-    <mergeCell ref="T80:X80"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="K27:O27"/>
+    <mergeCell ref="K36:O36"/>
+    <mergeCell ref="K63:O63"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="K144:O144"/>
+    <mergeCell ref="K152:O152"/>
+    <mergeCell ref="K160:O160"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="K75:O75"/>
+    <mergeCell ref="K127:O127"/>
+    <mergeCell ref="K136:O136"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28928,13 +28873,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.15">
       <c r="K4" s="2" t="s">
@@ -29073,13 +29018,13 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
       <c r="K14" s="4" t="s">
         <v>268</v>
       </c>
@@ -29266,13 +29211,13 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
       <c r="K23" s="4" t="s">
         <v>269</v>
       </c>
@@ -30363,13 +30308,13 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="K72" s="9" t="s">
+      <c r="K72" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="L72" s="10"/>
-      <c r="M72" s="10"/>
-      <c r="N72" s="10"/>
-      <c r="O72" s="11"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="15"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B73" s="2" t="s">
@@ -30532,20 +30477,20 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="K80" s="9" t="s">
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="K80" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="L80" s="10"/>
-      <c r="M80" s="10"/>
-      <c r="N80" s="10"/>
-      <c r="O80" s="11"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
+      <c r="N80" s="14"/>
+      <c r="O80" s="15"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B81" s="2" t="s">
@@ -30725,20 +30670,20 @@
       </c>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
-      <c r="K89" s="9" t="s">
+      <c r="C89" s="16"/>
+      <c r="D89" s="16"/>
+      <c r="E89" s="16"/>
+      <c r="F89" s="16"/>
+      <c r="K89" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="L89" s="10"/>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10"/>
-      <c r="O89" s="11"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="14"/>
+      <c r="N89" s="14"/>
+      <c r="O89" s="15"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B90" s="2" t="s">
@@ -30986,20 +30931,20 @@
       </c>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B102" s="12" t="s">
+      <c r="B102" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="K102" s="9" t="s">
+      <c r="C102" s="16"/>
+      <c r="D102" s="16"/>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
+      <c r="K102" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="L102" s="10"/>
-      <c r="M102" s="10"/>
-      <c r="N102" s="10"/>
-      <c r="O102" s="11"/>
+      <c r="L102" s="14"/>
+      <c r="M102" s="14"/>
+      <c r="N102" s="14"/>
+      <c r="O102" s="15"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B103" s="2" t="s">
@@ -31162,20 +31107,20 @@
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B110" s="9" t="s">
+      <c r="B110" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
-      <c r="E110" s="10"/>
-      <c r="F110" s="11"/>
-      <c r="K110" s="9" t="s">
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="15"/>
+      <c r="K110" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="L110" s="10"/>
-      <c r="M110" s="10"/>
-      <c r="N110" s="10"/>
-      <c r="O110" s="11"/>
+      <c r="L110" s="14"/>
+      <c r="M110" s="14"/>
+      <c r="N110" s="14"/>
+      <c r="O110" s="15"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B111" s="2" t="s">
@@ -31372,20 +31317,20 @@
       </c>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B120" s="9" t="s">
+      <c r="B120" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="C120" s="10"/>
-      <c r="D120" s="10"/>
-      <c r="E120" s="10"/>
-      <c r="F120" s="11"/>
-      <c r="K120" s="9" t="s">
+      <c r="C120" s="14"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="15"/>
+      <c r="K120" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="L120" s="10"/>
-      <c r="M120" s="10"/>
-      <c r="N120" s="10"/>
-      <c r="O120" s="11"/>
+      <c r="L120" s="14"/>
+      <c r="M120" s="14"/>
+      <c r="N120" s="14"/>
+      <c r="O120" s="15"/>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B121" s="2" t="s">
@@ -31565,20 +31510,20 @@
       </c>
     </row>
     <row r="129" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B129" s="9" t="s">
+      <c r="B129" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="10"/>
-      <c r="F129" s="11"/>
-      <c r="K129" s="9" t="s">
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14"/>
+      <c r="F129" s="15"/>
+      <c r="K129" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="L129" s="10"/>
-      <c r="M129" s="10"/>
-      <c r="N129" s="10"/>
-      <c r="O129" s="11"/>
+      <c r="L129" s="14"/>
+      <c r="M129" s="14"/>
+      <c r="N129" s="14"/>
+      <c r="O129" s="15"/>
     </row>
     <row r="130" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B130" s="2" t="s">
@@ -31758,20 +31703,20 @@
       </c>
     </row>
     <row r="138" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B138" s="12" t="s">
+      <c r="B138" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="C138" s="12"/>
-      <c r="D138" s="12"/>
-      <c r="E138" s="12"/>
-      <c r="F138" s="12"/>
-      <c r="K138" s="9" t="s">
+      <c r="C138" s="16"/>
+      <c r="D138" s="16"/>
+      <c r="E138" s="16"/>
+      <c r="F138" s="16"/>
+      <c r="K138" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="L138" s="10"/>
-      <c r="M138" s="10"/>
-      <c r="N138" s="10"/>
-      <c r="O138" s="11"/>
+      <c r="L138" s="14"/>
+      <c r="M138" s="14"/>
+      <c r="N138" s="14"/>
+      <c r="O138" s="15"/>
     </row>
     <row r="139" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B139" s="2" t="s">
@@ -31951,20 +31896,20 @@
       </c>
     </row>
     <row r="147" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B147" s="12" t="s">
+      <c r="B147" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="C147" s="12"/>
-      <c r="D147" s="12"/>
-      <c r="E147" s="12"/>
-      <c r="F147" s="12"/>
-      <c r="K147" s="9" t="s">
+      <c r="C147" s="16"/>
+      <c r="D147" s="16"/>
+      <c r="E147" s="16"/>
+      <c r="F147" s="16"/>
+      <c r="K147" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="L147" s="10"/>
-      <c r="M147" s="10"/>
-      <c r="N147" s="10"/>
-      <c r="O147" s="11"/>
+      <c r="L147" s="14"/>
+      <c r="M147" s="14"/>
+      <c r="N147" s="14"/>
+      <c r="O147" s="15"/>
     </row>
     <row r="148" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B148" s="2" t="s">
@@ -32127,20 +32072,20 @@
       </c>
     </row>
     <row r="155" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B155" s="9" t="s">
+      <c r="B155" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="C155" s="10"/>
-      <c r="D155" s="10"/>
-      <c r="E155" s="10"/>
-      <c r="F155" s="11"/>
-      <c r="K155" s="9" t="s">
+      <c r="C155" s="14"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
+      <c r="F155" s="15"/>
+      <c r="K155" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="L155" s="10"/>
-      <c r="M155" s="10"/>
-      <c r="N155" s="10"/>
-      <c r="O155" s="11"/>
+      <c r="L155" s="14"/>
+      <c r="M155" s="14"/>
+      <c r="N155" s="14"/>
+      <c r="O155" s="15"/>
     </row>
     <row r="156" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B156" s="2" t="s">
@@ -33026,13 +32971,13 @@
       </c>
     </row>
     <row r="197" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B197" s="9" t="s">
+      <c r="B197" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="C197" s="10"/>
-      <c r="D197" s="10"/>
-      <c r="E197" s="10"/>
-      <c r="F197" s="11"/>
+      <c r="C197" s="14"/>
+      <c r="D197" s="14"/>
+      <c r="E197" s="14"/>
+      <c r="F197" s="15"/>
       <c r="K197" s="4" t="s">
         <v>331</v>
       </c>
@@ -34046,13 +33991,13 @@
       </c>
     </row>
     <row r="254" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B254" s="12" t="s">
+      <c r="B254" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="C254" s="12"/>
-      <c r="D254" s="12"/>
-      <c r="E254" s="12"/>
-      <c r="F254" s="12"/>
+      <c r="C254" s="16"/>
+      <c r="D254" s="16"/>
+      <c r="E254" s="16"/>
+      <c r="F254" s="16"/>
       <c r="K254" s="4" t="s">
         <v>351</v>
       </c>
@@ -34477,13 +34422,13 @@
       </c>
     </row>
     <row r="278" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B278" s="9" t="s">
+      <c r="B278" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="C278" s="10"/>
-      <c r="D278" s="10"/>
-      <c r="E278" s="10"/>
-      <c r="F278" s="11"/>
+      <c r="C278" s="14"/>
+      <c r="D278" s="14"/>
+      <c r="E278" s="14"/>
+      <c r="F278" s="15"/>
       <c r="K278" s="4" t="s">
         <v>362</v>
       </c>
@@ -35022,13 +34967,13 @@
       </c>
     </row>
     <row r="303" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B303" s="9" t="s">
+      <c r="B303" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="C303" s="10"/>
-      <c r="D303" s="10"/>
-      <c r="E303" s="10"/>
-      <c r="F303" s="11"/>
+      <c r="C303" s="14"/>
+      <c r="D303" s="14"/>
+      <c r="E303" s="14"/>
+      <c r="F303" s="15"/>
       <c r="K303" s="4" t="s">
         <v>374</v>
       </c>
@@ -35567,13 +35512,13 @@
       </c>
     </row>
     <row r="328" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B328" s="9" t="s">
+      <c r="B328" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="C328" s="10"/>
-      <c r="D328" s="10"/>
-      <c r="E328" s="10"/>
-      <c r="F328" s="11"/>
+      <c r="C328" s="14"/>
+      <c r="D328" s="14"/>
+      <c r="E328" s="14"/>
+      <c r="F328" s="15"/>
       <c r="K328" s="4" t="s">
         <v>383</v>
       </c>
@@ -36080,13 +36025,13 @@
       </c>
     </row>
     <row r="352" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B352" s="9" t="s">
+      <c r="B352" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="C352" s="10"/>
-      <c r="D352" s="10"/>
-      <c r="E352" s="10"/>
-      <c r="F352" s="11"/>
+      <c r="C352" s="14"/>
+      <c r="D352" s="14"/>
+      <c r="E352" s="14"/>
+      <c r="F352" s="15"/>
       <c r="K352" s="4" t="s">
         <v>391</v>
       </c>
@@ -36593,29 +36538,29 @@
       </c>
     </row>
     <row r="375" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B375" s="14"/>
-      <c r="C375" s="14"/>
-      <c r="D375" s="14"/>
-      <c r="E375" s="14"/>
-      <c r="F375" s="14"/>
-      <c r="G375" s="14"/>
-      <c r="H375" s="14"/>
-      <c r="I375" s="14"/>
-      <c r="J375" s="14"/>
-      <c r="K375" s="14"/>
-      <c r="L375" s="14"/>
-      <c r="M375" s="14"/>
-      <c r="N375" s="14"/>
-      <c r="O375" s="14"/>
+      <c r="B375" s="9"/>
+      <c r="C375" s="9"/>
+      <c r="D375" s="9"/>
+      <c r="E375" s="9"/>
+      <c r="F375" s="9"/>
+      <c r="G375" s="9"/>
+      <c r="H375" s="9"/>
+      <c r="I375" s="9"/>
+      <c r="J375" s="9"/>
+      <c r="K375" s="9"/>
+      <c r="L375" s="9"/>
+      <c r="M375" s="9"/>
+      <c r="N375" s="9"/>
+      <c r="O375" s="9"/>
     </row>
     <row r="376" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B376" s="9" t="s">
+      <c r="B376" s="13" t="s">
         <v>397</v>
       </c>
-      <c r="C376" s="10"/>
-      <c r="D376" s="10"/>
-      <c r="E376" s="10"/>
-      <c r="F376" s="11"/>
+      <c r="C376" s="14"/>
+      <c r="D376" s="14"/>
+      <c r="E376" s="14"/>
+      <c r="F376" s="15"/>
       <c r="K376" s="4" t="s">
         <v>407</v>
       </c>
@@ -37348,6 +37293,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="K147:O147"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="K155:O155"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="K120:O120"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="K129:O129"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="K138:O138"/>
     <mergeCell ref="B376:F376"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="K3:O3"/>
@@ -37364,19 +37322,6 @@
     <mergeCell ref="B110:F110"/>
     <mergeCell ref="K110:O110"/>
     <mergeCell ref="B120:F120"/>
-    <mergeCell ref="K120:O120"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="K129:O129"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="K138:O138"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="K147:O147"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="K155:O155"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B278:F278"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37385,10 +37330,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7817DB2-39F5-448B-B4B5-837B004805D3}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B3:AP407"/>
+  <dimension ref="B3:AP401"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AC144" sqref="AC144"/>
+    <sheetView tabSelected="1" topLeftCell="L13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -37424,13 +37369,13 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
     </row>
     <row r="4" spans="2:42" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
@@ -37516,7 +37461,7 @@
         <v>24</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>5</v>
+        <v>476</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>23</v>
@@ -37542,7 +37487,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="3">
-        <v>100</v>
+        <v>255</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>3</v>
@@ -37774,7 +37719,7 @@
         <v>7</v>
       </c>
       <c r="F15" s="3">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>63</v>
@@ -38107,13 +38052,13 @@
         <v>5</v>
       </c>
       <c r="V20" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="W20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="X20" s="3">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="AC20" s="3" t="s">
         <v>448</v>
@@ -38276,7 +38221,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="3">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="AC23" s="3" t="s">
         <v>11</v>
@@ -38364,13 +38309,13 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="6"/>
-      <c r="T25" s="12" t="s">
+      <c r="T25" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="U25" s="12"/>
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
       <c r="AL25" s="3" t="s">
         <v>442</v>
       </c>
@@ -38458,19 +38403,19 @@
         <v>15</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>418</v>
+        <v>24</v>
       </c>
       <c r="U27" s="3" t="s">
-        <v>17</v>
+        <v>271</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="X27" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="X27" s="3">
+        <v>15</v>
       </c>
       <c r="AC27" s="2" t="s">
         <v>26</v>
@@ -38527,19 +38472,19 @@
         <v>5</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>270</v>
+        <v>476</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="W28" s="3" t="s">
         <v>7</v>
       </c>
       <c r="X28" s="3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="AC28" s="3" t="s">
         <v>418</v>
@@ -38589,7 +38534,7 @@
         <v>5</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U29" s="3" t="s">
         <v>5</v>
@@ -38601,7 +38546,7 @@
         <v>7</v>
       </c>
       <c r="X29" s="3">
-        <v>50</v>
+        <v>255</v>
       </c>
       <c r="AC29" s="3" t="s">
         <v>442</v>
@@ -38651,19 +38596,19 @@
         <v>5</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="U30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="V30" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="X30" s="3">
-        <v>255</v>
+        <v>10</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="AC30" s="3" t="s">
         <v>448</v>
@@ -38702,7 +38647,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="3">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>9</v>
@@ -38720,13 +38665,13 @@
         <v>5</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="U31" s="3" t="s">
         <v>5</v>
       </c>
       <c r="V31" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="W31" s="3" t="s">
         <v>10</v>
@@ -38794,21 +38739,6 @@
         <v>10</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="T32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="V32" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="X32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AC32" s="3" t="s">
@@ -39113,7 +39043,7 @@
         <v>7</v>
       </c>
       <c r="F39" s="3">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>69</v>
@@ -39372,11 +39302,11 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="16"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
-      <c r="O44" s="16"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
       <c r="T44" s="1" t="s">
         <v>267</v>
       </c>
@@ -39408,11 +39338,6 @@
       <c r="F45" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
       <c r="T45" s="2" t="s">
         <v>26</v>
       </c>
@@ -39460,11 +39385,6 @@
       <c r="F46" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
       <c r="T46" s="3" t="s">
         <v>418</v>
       </c>
@@ -39519,11 +39439,6 @@
       <c r="F47" s="3">
         <v>50</v>
       </c>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
       <c r="T47" s="3" t="s">
         <v>442</v>
       </c>
@@ -39586,11 +39501,6 @@
       <c r="F48" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
       <c r="T48" s="3" t="s">
         <v>9</v>
       </c>
@@ -39653,11 +39563,6 @@
       <c r="F49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
       <c r="T49" s="3" t="s">
         <v>11</v>
       </c>
@@ -39705,11 +39610,6 @@
       </c>
     </row>
     <row r="50" spans="2:42" x14ac:dyDescent="0.15">
-      <c r="K50" s="15"/>
-      <c r="L50" s="15"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="15"/>
-      <c r="O50" s="15"/>
       <c r="AC50" s="3" t="s">
         <v>448</v>
       </c>
@@ -39742,11 +39642,6 @@
       </c>
     </row>
     <row r="51" spans="2:42" x14ac:dyDescent="0.15">
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
       <c r="AC51" s="3" t="s">
         <v>451</v>
       </c>
@@ -39955,7 +39850,7 @@
         <v>309</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N55" s="3" t="s">
         <v>4</v>
@@ -40017,7 +39912,7 @@
         <v>312</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N56" s="3" t="s">
         <v>4</v>
@@ -40038,7 +39933,7 @@
         <v>7</v>
       </c>
       <c r="X56" s="3">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="AC56" s="1" t="s">
         <v>462</v>
@@ -40304,13 +40199,13 @@
       <c r="F61" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K61" s="12" t="s">
+      <c r="K61" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="L61" s="12"/>
-      <c r="M61" s="12"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="12"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
       <c r="T61" s="3" t="s">
         <v>51</v>
       </c>
@@ -40324,7 +40219,7 @@
         <v>7</v>
       </c>
       <c r="X61" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="AC61" s="3" t="s">
         <v>451</v>
@@ -40434,7 +40329,7 @@
         <v>270</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N63" s="3" t="s">
         <v>7</v>
@@ -40511,7 +40406,7 @@
         <v>343</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N64" s="3" t="s">
         <v>4</v>
@@ -40573,7 +40468,7 @@
         <v>270</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N65" s="3" t="s">
         <v>7</v>
@@ -40801,7 +40696,7 @@
     </row>
     <row r="70" spans="2:42" x14ac:dyDescent="0.15">
       <c r="B70" s="4" t="s">
-        <v>303</v>
+        <v>475</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -40854,13 +40749,13 @@
       <c r="F71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K71" s="9" t="s">
+      <c r="K71" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="L71" s="10"/>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10"/>
-      <c r="O71" s="11"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="14"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="15"/>
       <c r="T71" s="3" t="s">
         <v>9</v>
       </c>
@@ -40994,7 +40889,7 @@
         <v>270</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N74" s="3" t="s">
         <v>7</v>
@@ -41033,7 +40928,7 @@
         <v>315</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N75" s="3" t="s">
         <v>4</v>
@@ -41072,7 +40967,7 @@
         <v>317</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N76" s="3" t="s">
         <v>4</v>
@@ -41119,7 +41014,7 @@
         <v>326</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N77" s="3" t="s">
         <v>4</v>
@@ -41173,7 +41068,7 @@
         <v>328</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N78" s="3" t="s">
         <v>4</v>
@@ -41495,7 +41390,7 @@
         <v>270</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N86" s="3" t="s">
         <v>7</v>
@@ -41542,7 +41437,7 @@
         <v>335</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N87" s="3" t="s">
         <v>4</v>
@@ -41589,7 +41484,7 @@
         <v>356</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N88" s="3" t="s">
         <v>4</v>
@@ -41813,13 +41708,13 @@
       </c>
     </row>
     <row r="95" spans="2:33" x14ac:dyDescent="0.15">
-      <c r="K95" s="9" t="s">
+      <c r="K95" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="L95" s="10"/>
-      <c r="M95" s="10"/>
-      <c r="N95" s="10"/>
-      <c r="O95" s="11"/>
+      <c r="L95" s="14"/>
+      <c r="M95" s="14"/>
+      <c r="N95" s="14"/>
+      <c r="O95" s="15"/>
       <c r="T95" s="3" t="s">
         <v>9</v>
       </c>
@@ -41930,7 +41825,7 @@
         <v>270</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N98" s="3" t="s">
         <v>7</v>
@@ -41962,7 +41857,7 @@
         <v>365</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N99" s="3" t="s">
         <v>4</v>
@@ -42001,7 +41896,7 @@
         <v>367</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N100" s="3" t="s">
         <v>4</v>
@@ -42045,7 +41940,7 @@
         <v>149</v>
       </c>
       <c r="L101" s="3" t="s">
-        <v>270</v>
+        <v>477</v>
       </c>
       <c r="M101" s="3" t="s">
         <v>19</v>
@@ -42238,11 +42133,6 @@
       <c r="F106" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T106" s="15"/>
-      <c r="U106" s="15"/>
-      <c r="V106" s="15"/>
-      <c r="W106" s="15"/>
-      <c r="X106" s="15"/>
     </row>
     <row r="107" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B107" s="3" t="s">
@@ -42260,11 +42150,11 @@
       <c r="F107" s="3">
         <v>50</v>
       </c>
-      <c r="T107" s="16"/>
-      <c r="U107" s="16"/>
-      <c r="V107" s="16"/>
-      <c r="W107" s="16"/>
-      <c r="X107" s="16"/>
+      <c r="T107" s="10"/>
+      <c r="U107" s="10"/>
+      <c r="V107" s="10"/>
+      <c r="W107" s="10"/>
+      <c r="X107" s="10"/>
     </row>
     <row r="108" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B108" s="3" t="s">
@@ -42282,13 +42172,13 @@
       <c r="F108" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K108" s="9" t="s">
+      <c r="K108" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="L108" s="10"/>
-      <c r="M108" s="10"/>
-      <c r="N108" s="10"/>
-      <c r="O108" s="11"/>
+      <c r="L108" s="14"/>
+      <c r="M108" s="14"/>
+      <c r="N108" s="14"/>
+      <c r="O108" s="15"/>
       <c r="T108" s="4" t="s">
         <v>422</v>
       </c>
@@ -42349,7 +42239,7 @@
         <v>437</v>
       </c>
       <c r="L110" s="3" t="s">
-        <v>270</v>
+        <v>477</v>
       </c>
       <c r="M110" s="3" t="s">
         <v>19</v>
@@ -42384,7 +42274,7 @@
         <v>378</v>
       </c>
       <c r="M111" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N111" s="3" t="s">
         <v>4</v>
@@ -42396,7 +42286,7 @@
         <v>189</v>
       </c>
       <c r="U111" s="3" t="s">
-        <v>270</v>
+        <v>477</v>
       </c>
       <c r="V111" s="3" t="s">
         <v>19</v>
@@ -42423,7 +42313,7 @@
         <v>379</v>
       </c>
       <c r="M112" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N112" s="3" t="s">
         <v>4</v>
@@ -42647,16 +42537,11 @@
       </c>
     </row>
     <row r="119" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="K119" s="15"/>
-      <c r="L119" s="15"/>
-      <c r="M119" s="15"/>
-      <c r="N119" s="15"/>
-      <c r="O119" s="15"/>
       <c r="T119" s="3" t="s">
         <v>99</v>
       </c>
       <c r="U119" s="3" t="s">
-        <v>270</v>
+        <v>477</v>
       </c>
       <c r="V119" s="3" t="s">
         <v>19</v>
@@ -42676,13 +42561,13 @@
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
       <c r="F120" s="6"/>
-      <c r="K120" s="9" t="s">
+      <c r="K120" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="L120" s="10"/>
-      <c r="M120" s="10"/>
-      <c r="N120" s="10"/>
-      <c r="O120" s="11"/>
+      <c r="L120" s="14"/>
+      <c r="M120" s="14"/>
+      <c r="N120" s="14"/>
+      <c r="O120" s="15"/>
       <c r="T120" s="3" t="s">
         <v>9</v>
       </c>
@@ -42769,7 +42654,7 @@
         <v>270</v>
       </c>
       <c r="M122" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N122" s="3" t="s">
         <v>7</v>
@@ -42801,7 +42686,7 @@
         <v>385</v>
       </c>
       <c r="M123" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N123" s="3" t="s">
         <v>4</v>
@@ -42833,7 +42718,7 @@
         <v>386</v>
       </c>
       <c r="M124" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N124" s="3" t="s">
         <v>4</v>
@@ -42933,7 +42818,7 @@
         <v>103</v>
       </c>
       <c r="U127" s="3" t="s">
-        <v>309</v>
+        <v>478</v>
       </c>
       <c r="V127" s="3" t="s">
         <v>19</v>
@@ -43017,13 +42902,13 @@
       <c r="F130" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K130" s="9" t="s">
+      <c r="K130" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="L130" s="10"/>
-      <c r="M130" s="10"/>
-      <c r="N130" s="10"/>
-      <c r="O130" s="11"/>
+      <c r="L130" s="14"/>
+      <c r="M130" s="14"/>
+      <c r="N130" s="14"/>
+      <c r="O130" s="15"/>
     </row>
     <row r="131" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B131" s="3" t="s">
@@ -43080,7 +42965,7 @@
         <v>270</v>
       </c>
       <c r="M132" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N132" s="3" t="s">
         <v>7</v>
@@ -43119,7 +43004,7 @@
         <v>396</v>
       </c>
       <c r="M133" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N133" s="3" t="s">
         <v>4</v>
@@ -43151,7 +43036,7 @@
         <v>395</v>
       </c>
       <c r="M134" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N134" s="3" t="s">
         <v>4</v>
@@ -43176,11 +43061,11 @@
       </c>
     </row>
     <row r="135" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B135" s="16"/>
-      <c r="C135" s="16"/>
-      <c r="D135" s="16"/>
-      <c r="E135" s="16"/>
-      <c r="F135" s="16"/>
+      <c r="B135" s="10"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+      <c r="F135" s="10"/>
       <c r="K135" s="3" t="s">
         <v>9</v>
       </c>
@@ -43348,13 +43233,13 @@
       <c r="F140" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K140" s="9" t="s">
+      <c r="K140" s="13" t="s">
         <v>397</v>
       </c>
-      <c r="L140" s="10"/>
-      <c r="M140" s="10"/>
-      <c r="N140" s="10"/>
-      <c r="O140" s="11"/>
+      <c r="L140" s="14"/>
+      <c r="M140" s="14"/>
+      <c r="N140" s="14"/>
+      <c r="O140" s="15"/>
     </row>
     <row r="141" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B141" s="3" t="s">
@@ -43403,7 +43288,7 @@
         <v>270</v>
       </c>
       <c r="M142" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N142" s="3" t="s">
         <v>7</v>
@@ -43435,7 +43320,7 @@
         <v>439</v>
       </c>
       <c r="M143" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N143" s="3" t="s">
         <v>4</v>
@@ -43474,7 +43359,7 @@
         <v>440</v>
       </c>
       <c r="M144" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N144" s="3" t="s">
         <v>4</v>
@@ -43486,7 +43371,7 @@
         <v>189</v>
       </c>
       <c r="U144" s="3" t="s">
-        <v>270</v>
+        <v>477</v>
       </c>
       <c r="V144" s="3" t="s">
         <v>19</v>
@@ -43756,7 +43641,7 @@
         <v>99</v>
       </c>
       <c r="U152" s="3" t="s">
-        <v>270</v>
+        <v>477</v>
       </c>
       <c r="V152" s="3" t="s">
         <v>19</v>
@@ -43848,11 +43733,11 @@
       <c r="F155" s="3">
         <v>50</v>
       </c>
-      <c r="K155" s="16"/>
-      <c r="L155" s="16"/>
-      <c r="M155" s="16"/>
-      <c r="N155" s="16"/>
-      <c r="O155" s="16"/>
+      <c r="K155" s="10"/>
+      <c r="L155" s="10"/>
+      <c r="M155" s="10"/>
+      <c r="N155" s="10"/>
+      <c r="O155" s="10"/>
     </row>
     <row r="156" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B156" s="3" t="s">
@@ -43887,11 +43772,6 @@
       <c r="F157" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K157" s="15"/>
-      <c r="L157" s="15"/>
-      <c r="M157" s="15"/>
-      <c r="N157" s="15"/>
-      <c r="O157" s="15"/>
       <c r="T157" s="4" t="s">
         <v>428</v>
       </c>
@@ -43901,11 +43781,6 @@
       <c r="X157" s="6"/>
     </row>
     <row r="158" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="K158" s="15"/>
-      <c r="L158" s="15"/>
-      <c r="M158" s="15"/>
-      <c r="N158" s="15"/>
-      <c r="O158" s="15"/>
       <c r="T158" s="2" t="s">
         <v>26</v>
       </c>
@@ -43951,7 +43826,7 @@
         <v>103</v>
       </c>
       <c r="U160" s="3" t="s">
-        <v>309</v>
+        <v>478</v>
       </c>
       <c r="V160" s="3" t="s">
         <v>19</v>
@@ -44627,783 +44502,149 @@
       </c>
     </row>
     <row r="211" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B211" s="16"/>
-      <c r="C211" s="16"/>
-      <c r="D211" s="16"/>
-      <c r="E211" s="16"/>
-      <c r="F211" s="16"/>
-    </row>
-    <row r="212" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B212" s="15"/>
-      <c r="C212" s="15"/>
-      <c r="D212" s="15"/>
-      <c r="E212" s="15"/>
-      <c r="F212" s="15"/>
-    </row>
-    <row r="213" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B213" s="15"/>
-      <c r="C213" s="15"/>
-      <c r="D213" s="15"/>
-      <c r="E213" s="15"/>
-      <c r="F213" s="15"/>
-    </row>
-    <row r="214" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B214" s="15"/>
-      <c r="C214" s="15"/>
-      <c r="D214" s="15"/>
-      <c r="E214" s="15"/>
-      <c r="F214" s="15"/>
-    </row>
-    <row r="215" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K215" s="15"/>
-      <c r="L215" s="15"/>
-      <c r="M215" s="15"/>
-      <c r="N215" s="15"/>
-      <c r="O215" s="15"/>
-    </row>
-    <row r="216" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K216" s="15"/>
-      <c r="L216" s="15"/>
-      <c r="M216" s="15"/>
-      <c r="N216" s="15"/>
-      <c r="O216" s="15"/>
-    </row>
-    <row r="217" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K217" s="15"/>
-      <c r="L217" s="15"/>
-      <c r="M217" s="15"/>
-      <c r="N217" s="15"/>
-      <c r="O217" s="15"/>
-    </row>
-    <row r="218" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K218" s="15"/>
-      <c r="L218" s="15"/>
-      <c r="M218" s="15"/>
-      <c r="N218" s="15"/>
-      <c r="O218" s="15"/>
-    </row>
-    <row r="219" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K219" s="15"/>
-      <c r="L219" s="15"/>
-      <c r="M219" s="15"/>
-      <c r="N219" s="15"/>
-      <c r="O219" s="15"/>
+      <c r="B211" s="10"/>
+      <c r="C211" s="10"/>
+      <c r="D211" s="10"/>
+      <c r="E211" s="10"/>
+      <c r="F211" s="10"/>
     </row>
     <row r="222" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K222" s="16"/>
-      <c r="L222" s="16"/>
-      <c r="M222" s="16"/>
-      <c r="N222" s="16"/>
-      <c r="O222" s="16"/>
-    </row>
-    <row r="223" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K223" s="15"/>
-      <c r="L223" s="15"/>
-      <c r="M223" s="15"/>
-      <c r="N223" s="15"/>
-      <c r="O223" s="15"/>
-    </row>
-    <row r="224" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K224" s="15"/>
-      <c r="L224" s="15"/>
-      <c r="M224" s="15"/>
-      <c r="N224" s="15"/>
-      <c r="O224" s="15"/>
-    </row>
-    <row r="225" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K225" s="15"/>
-      <c r="L225" s="15"/>
-      <c r="M225" s="15"/>
-      <c r="N225" s="15"/>
-      <c r="O225" s="15"/>
-    </row>
-    <row r="226" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K226" s="15"/>
-      <c r="L226" s="15"/>
-      <c r="M226" s="15"/>
-      <c r="N226" s="15"/>
-      <c r="O226" s="15"/>
-    </row>
-    <row r="235" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K235" s="15"/>
-      <c r="L235" s="15"/>
-      <c r="M235" s="15"/>
-      <c r="N235" s="15"/>
-      <c r="O235" s="15"/>
+      <c r="K222" s="10"/>
+      <c r="L222" s="10"/>
+      <c r="M222" s="10"/>
+      <c r="N222" s="10"/>
+      <c r="O222" s="10"/>
     </row>
     <row r="239" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K239" s="17"/>
-      <c r="L239" s="17"/>
-      <c r="M239" s="17"/>
-      <c r="N239" s="17"/>
-      <c r="O239" s="17"/>
+      <c r="K239" s="11"/>
+      <c r="L239" s="11"/>
+      <c r="M239" s="11"/>
+      <c r="N239" s="11"/>
+      <c r="O239" s="11"/>
     </row>
     <row r="240" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K240" s="17"/>
-      <c r="L240" s="17"/>
-      <c r="M240" s="17"/>
-      <c r="N240" s="17"/>
-      <c r="O240" s="17"/>
+      <c r="K240" s="11"/>
+      <c r="L240" s="11"/>
+      <c r="M240" s="11"/>
+      <c r="N240" s="11"/>
+      <c r="O240" s="11"/>
     </row>
     <row r="241" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K241" s="17"/>
-      <c r="L241" s="17"/>
-      <c r="M241" s="17"/>
-      <c r="N241" s="17"/>
-      <c r="O241" s="17"/>
-    </row>
-    <row r="304" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K304" s="15"/>
-      <c r="L304" s="15"/>
-      <c r="M304" s="15"/>
-      <c r="N304" s="15"/>
-      <c r="O304" s="15"/>
-    </row>
-    <row r="305" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K305" s="15"/>
-      <c r="L305" s="15"/>
-      <c r="M305" s="15"/>
-      <c r="N305" s="15"/>
-      <c r="O305" s="15"/>
-    </row>
-    <row r="306" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K306" s="15"/>
-      <c r="L306" s="15"/>
-      <c r="M306" s="15"/>
-      <c r="N306" s="15"/>
-      <c r="O306" s="15"/>
-    </row>
-    <row r="307" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K307" s="15"/>
-      <c r="L307" s="15"/>
-      <c r="M307" s="15"/>
-      <c r="N307" s="15"/>
-      <c r="O307" s="15"/>
-    </row>
-    <row r="308" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K308" s="15"/>
-      <c r="L308" s="15"/>
-      <c r="M308" s="15"/>
-      <c r="N308" s="15"/>
-      <c r="O308" s="15"/>
-    </row>
-    <row r="309" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K309" s="15"/>
-      <c r="L309" s="15"/>
-      <c r="M309" s="15"/>
-      <c r="N309" s="15"/>
-      <c r="O309" s="15"/>
-    </row>
-    <row r="310" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K310" s="15"/>
-      <c r="L310" s="15"/>
-      <c r="M310" s="15"/>
-      <c r="N310" s="15"/>
-      <c r="O310" s="15"/>
-    </row>
-    <row r="311" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K311" s="15"/>
-      <c r="L311" s="15"/>
-      <c r="M311" s="15"/>
-      <c r="N311" s="15"/>
-      <c r="O311" s="15"/>
+      <c r="K241" s="11"/>
+      <c r="L241" s="11"/>
+      <c r="M241" s="11"/>
+      <c r="N241" s="11"/>
+      <c r="O241" s="11"/>
     </row>
     <row r="312" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K312" s="16"/>
-      <c r="L312" s="16"/>
-      <c r="M312" s="16"/>
-      <c r="N312" s="16"/>
-      <c r="O312" s="16"/>
+      <c r="K312" s="10"/>
+      <c r="L312" s="10"/>
+      <c r="M312" s="10"/>
+      <c r="N312" s="10"/>
+      <c r="O312" s="10"/>
     </row>
     <row r="328" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K328" s="16"/>
-      <c r="L328" s="16"/>
-      <c r="M328" s="16"/>
-      <c r="N328" s="16"/>
-      <c r="O328" s="16"/>
-    </row>
-    <row r="329" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K329" s="15"/>
-      <c r="L329" s="15"/>
-      <c r="M329" s="15"/>
-      <c r="N329" s="15"/>
-      <c r="O329" s="15"/>
-    </row>
-    <row r="330" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K330" s="15"/>
-      <c r="L330" s="15"/>
-      <c r="M330" s="15"/>
-      <c r="N330" s="15"/>
-      <c r="O330" s="15"/>
-    </row>
-    <row r="331" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K331" s="15"/>
-      <c r="L331" s="15"/>
-      <c r="M331" s="15"/>
-      <c r="N331" s="15"/>
-      <c r="O331" s="15"/>
-    </row>
-    <row r="332" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K332" s="15"/>
-      <c r="L332" s="15"/>
-      <c r="M332" s="15"/>
-      <c r="N332" s="15"/>
-      <c r="O332" s="15"/>
-    </row>
-    <row r="333" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K333" s="15"/>
-      <c r="L333" s="15"/>
-      <c r="M333" s="15"/>
-      <c r="N333" s="15"/>
-      <c r="O333" s="15"/>
-    </row>
-    <row r="334" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K334" s="15"/>
-      <c r="L334" s="15"/>
-      <c r="M334" s="15"/>
-      <c r="N334" s="15"/>
-      <c r="O334" s="15"/>
-    </row>
-    <row r="335" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K335" s="15"/>
-      <c r="L335" s="15"/>
-      <c r="M335" s="15"/>
-      <c r="N335" s="15"/>
-      <c r="O335" s="15"/>
+      <c r="K328" s="10"/>
+      <c r="L328" s="10"/>
+      <c r="M328" s="10"/>
+      <c r="N328" s="10"/>
+      <c r="O328" s="10"/>
     </row>
     <row r="336" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K336" s="16"/>
-      <c r="L336" s="16"/>
-      <c r="M336" s="16"/>
-      <c r="N336" s="16"/>
-      <c r="O336" s="16"/>
-    </row>
-    <row r="337" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K337" s="15"/>
-      <c r="L337" s="15"/>
-      <c r="M337" s="15"/>
-      <c r="N337" s="15"/>
-      <c r="O337" s="15"/>
-    </row>
-    <row r="338" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K338" s="15"/>
-      <c r="L338" s="15"/>
-      <c r="M338" s="15"/>
-      <c r="N338" s="15"/>
-      <c r="O338" s="15"/>
-    </row>
-    <row r="339" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K339" s="15"/>
-      <c r="L339" s="15"/>
-      <c r="M339" s="15"/>
-      <c r="N339" s="15"/>
-      <c r="O339" s="15"/>
-    </row>
-    <row r="340" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K340" s="15"/>
-      <c r="L340" s="15"/>
-      <c r="M340" s="15"/>
-      <c r="N340" s="15"/>
-      <c r="O340" s="15"/>
-    </row>
-    <row r="341" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K341" s="15"/>
-      <c r="L341" s="15"/>
-      <c r="M341" s="15"/>
-      <c r="N341" s="15"/>
-      <c r="O341" s="15"/>
-    </row>
-    <row r="342" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K342" s="15"/>
-      <c r="L342" s="15"/>
-      <c r="M342" s="15"/>
-      <c r="N342" s="15"/>
-      <c r="O342" s="15"/>
-    </row>
-    <row r="343" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K343" s="15"/>
-      <c r="L343" s="15"/>
-      <c r="M343" s="15"/>
-      <c r="N343" s="15"/>
-      <c r="O343" s="15"/>
+      <c r="K336" s="10"/>
+      <c r="L336" s="10"/>
+      <c r="M336" s="10"/>
+      <c r="N336" s="10"/>
+      <c r="O336" s="10"/>
     </row>
     <row r="344" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K344" s="16"/>
-      <c r="L344" s="16"/>
-      <c r="M344" s="16"/>
-      <c r="N344" s="16"/>
-      <c r="O344" s="16"/>
-    </row>
-    <row r="345" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K345" s="15"/>
-      <c r="L345" s="15"/>
-      <c r="M345" s="15"/>
-      <c r="N345" s="15"/>
-      <c r="O345" s="15"/>
-    </row>
-    <row r="346" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K346" s="15"/>
-      <c r="L346" s="15"/>
-      <c r="M346" s="15"/>
-      <c r="N346" s="15"/>
-      <c r="O346" s="15"/>
-    </row>
-    <row r="347" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K347" s="15"/>
-      <c r="L347" s="15"/>
-      <c r="M347" s="15"/>
-      <c r="N347" s="15"/>
-      <c r="O347" s="15"/>
-    </row>
-    <row r="348" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K348" s="15"/>
-      <c r="L348" s="15"/>
-      <c r="M348" s="15"/>
-      <c r="N348" s="15"/>
-      <c r="O348" s="15"/>
-    </row>
-    <row r="349" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K349" s="15"/>
-      <c r="L349" s="15"/>
-      <c r="M349" s="15"/>
-      <c r="N349" s="15"/>
-      <c r="O349" s="15"/>
+      <c r="K344" s="10"/>
+      <c r="L344" s="10"/>
+      <c r="M344" s="10"/>
+      <c r="N344" s="10"/>
+      <c r="O344" s="10"/>
     </row>
     <row r="352" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K352" s="16"/>
-      <c r="L352" s="16"/>
-      <c r="M352" s="16"/>
-      <c r="N352" s="16"/>
-      <c r="O352" s="16"/>
-    </row>
-    <row r="353" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K353" s="15"/>
-      <c r="L353" s="15"/>
-      <c r="M353" s="15"/>
-      <c r="N353" s="15"/>
-      <c r="O353" s="15"/>
-    </row>
-    <row r="354" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K354" s="15"/>
-      <c r="L354" s="15"/>
-      <c r="M354" s="15"/>
-      <c r="N354" s="15"/>
-      <c r="O354" s="15"/>
-    </row>
-    <row r="355" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K355" s="15"/>
-      <c r="L355" s="15"/>
-      <c r="M355" s="15"/>
-      <c r="N355" s="15"/>
-      <c r="O355" s="15"/>
-    </row>
-    <row r="356" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K356" s="15"/>
-      <c r="L356" s="15"/>
-      <c r="M356" s="15"/>
-      <c r="N356" s="15"/>
-      <c r="O356" s="15"/>
-    </row>
-    <row r="357" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K357" s="15"/>
-      <c r="L357" s="15"/>
-      <c r="M357" s="15"/>
-      <c r="N357" s="15"/>
-      <c r="O357" s="15"/>
-    </row>
-    <row r="358" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K358" s="15"/>
-      <c r="L358" s="15"/>
-      <c r="M358" s="15"/>
-      <c r="N358" s="15"/>
-      <c r="O358" s="15"/>
-    </row>
-    <row r="359" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K359" s="15"/>
-      <c r="L359" s="15"/>
-      <c r="M359" s="15"/>
-      <c r="N359" s="15"/>
-      <c r="O359" s="15"/>
+      <c r="K352" s="10"/>
+      <c r="L352" s="10"/>
+      <c r="M352" s="10"/>
+      <c r="N352" s="10"/>
+      <c r="O352" s="10"/>
     </row>
     <row r="360" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K360" s="16"/>
-      <c r="L360" s="16"/>
-      <c r="M360" s="16"/>
-      <c r="N360" s="16"/>
-      <c r="O360" s="16"/>
-    </row>
-    <row r="361" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K361" s="15"/>
-      <c r="L361" s="15"/>
-      <c r="M361" s="15"/>
-      <c r="N361" s="15"/>
-      <c r="O361" s="15"/>
-    </row>
-    <row r="362" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K362" s="15"/>
-      <c r="L362" s="15"/>
-      <c r="M362" s="15"/>
-      <c r="N362" s="15"/>
-      <c r="O362" s="15"/>
-    </row>
-    <row r="363" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K363" s="15"/>
-      <c r="L363" s="15"/>
-      <c r="M363" s="15"/>
-      <c r="N363" s="15"/>
-      <c r="O363" s="15"/>
-    </row>
-    <row r="364" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K364" s="15"/>
-      <c r="L364" s="15"/>
-      <c r="M364" s="15"/>
-      <c r="N364" s="15"/>
-      <c r="O364" s="15"/>
-    </row>
-    <row r="365" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K365" s="15"/>
-      <c r="L365" s="15"/>
-      <c r="M365" s="15"/>
-      <c r="N365" s="15"/>
-      <c r="O365" s="15"/>
-    </row>
-    <row r="366" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K366" s="15"/>
-      <c r="L366" s="15"/>
-      <c r="M366" s="15"/>
-      <c r="N366" s="15"/>
-      <c r="O366" s="15"/>
-    </row>
-    <row r="367" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K367" s="15"/>
-      <c r="L367" s="15"/>
-      <c r="M367" s="15"/>
-      <c r="N367" s="15"/>
-      <c r="O367" s="15"/>
+      <c r="K360" s="10"/>
+      <c r="L360" s="10"/>
+      <c r="M360" s="10"/>
+      <c r="N360" s="10"/>
+      <c r="O360" s="10"/>
     </row>
     <row r="368" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K368" s="16"/>
-      <c r="L368" s="16"/>
-      <c r="M368" s="16"/>
-      <c r="N368" s="16"/>
-      <c r="O368" s="16"/>
-    </row>
-    <row r="369" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K369" s="15"/>
-      <c r="L369" s="15"/>
-      <c r="M369" s="15"/>
-      <c r="N369" s="15"/>
-      <c r="O369" s="15"/>
-    </row>
-    <row r="370" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K370" s="15"/>
-      <c r="L370" s="15"/>
-      <c r="M370" s="15"/>
-      <c r="N370" s="15"/>
-      <c r="O370" s="15"/>
-    </row>
-    <row r="371" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K371" s="15"/>
-      <c r="L371" s="15"/>
-      <c r="M371" s="15"/>
-      <c r="N371" s="15"/>
-      <c r="O371" s="15"/>
-    </row>
-    <row r="372" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K372" s="15"/>
-      <c r="L372" s="15"/>
-      <c r="M372" s="15"/>
-      <c r="N372" s="15"/>
-      <c r="O372" s="15"/>
-    </row>
-    <row r="373" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K373" s="15"/>
-      <c r="L373" s="15"/>
-      <c r="M373" s="15"/>
-      <c r="N373" s="15"/>
-      <c r="O373" s="15"/>
+      <c r="K368" s="10"/>
+      <c r="L368" s="10"/>
+      <c r="M368" s="10"/>
+      <c r="N368" s="10"/>
+      <c r="O368" s="10"/>
     </row>
     <row r="375" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B375" s="18"/>
-      <c r="C375" s="18"/>
-      <c r="D375" s="18"/>
-      <c r="E375" s="18"/>
-      <c r="F375" s="18"/>
-      <c r="G375" s="18"/>
-      <c r="H375" s="18"/>
-      <c r="I375" s="18"/>
-      <c r="J375" s="18"/>
-      <c r="K375" s="18"/>
-      <c r="L375" s="18"/>
-      <c r="M375" s="18"/>
-      <c r="N375" s="18"/>
-      <c r="O375" s="18"/>
+      <c r="B375" s="12"/>
+      <c r="C375" s="12"/>
+      <c r="D375" s="12"/>
+      <c r="E375" s="12"/>
+      <c r="F375" s="12"/>
+      <c r="G375" s="12"/>
+      <c r="H375" s="12"/>
+      <c r="I375" s="12"/>
+      <c r="J375" s="12"/>
+      <c r="K375" s="12"/>
+      <c r="L375" s="12"/>
+      <c r="M375" s="12"/>
+      <c r="N375" s="12"/>
+      <c r="O375" s="12"/>
     </row>
     <row r="376" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K376" s="16"/>
-      <c r="L376" s="16"/>
-      <c r="M376" s="16"/>
-      <c r="N376" s="16"/>
-      <c r="O376" s="16"/>
-    </row>
-    <row r="377" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K377" s="15"/>
-      <c r="L377" s="15"/>
-      <c r="M377" s="15"/>
-      <c r="N377" s="15"/>
-      <c r="O377" s="15"/>
-    </row>
-    <row r="378" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K378" s="15"/>
-      <c r="L378" s="15"/>
-      <c r="M378" s="15"/>
-      <c r="N378" s="15"/>
-      <c r="O378" s="15"/>
-    </row>
-    <row r="379" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K379" s="15"/>
-      <c r="L379" s="15"/>
-      <c r="M379" s="15"/>
-      <c r="N379" s="15"/>
-      <c r="O379" s="15"/>
-    </row>
-    <row r="380" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K380" s="15"/>
-      <c r="L380" s="15"/>
-      <c r="M380" s="15"/>
-      <c r="N380" s="15"/>
-      <c r="O380" s="15"/>
-    </row>
-    <row r="381" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K381" s="15"/>
-      <c r="L381" s="15"/>
-      <c r="M381" s="15"/>
-      <c r="N381" s="15"/>
-      <c r="O381" s="15"/>
-    </row>
-    <row r="382" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K382" s="15"/>
-      <c r="L382" s="15"/>
-      <c r="M382" s="15"/>
-      <c r="N382" s="15"/>
-      <c r="O382" s="15"/>
-    </row>
-    <row r="383" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K383" s="15"/>
-      <c r="L383" s="15"/>
-      <c r="M383" s="15"/>
-      <c r="N383" s="15"/>
-      <c r="O383" s="15"/>
-    </row>
-    <row r="384" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="K384" s="15"/>
-      <c r="L384" s="15"/>
-      <c r="M384" s="15"/>
-      <c r="N384" s="15"/>
-      <c r="O384" s="15"/>
+      <c r="K376" s="10"/>
+      <c r="L376" s="10"/>
+      <c r="M376" s="10"/>
+      <c r="N376" s="10"/>
+      <c r="O376" s="10"/>
     </row>
     <row r="385" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K385" s="16"/>
-      <c r="L385" s="16"/>
-      <c r="M385" s="16"/>
-      <c r="N385" s="16"/>
-      <c r="O385" s="16"/>
-    </row>
-    <row r="386" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K386" s="15"/>
-      <c r="L386" s="15"/>
-      <c r="M386" s="15"/>
-      <c r="N386" s="15"/>
-      <c r="O386" s="15"/>
-    </row>
-    <row r="387" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K387" s="15"/>
-      <c r="L387" s="15"/>
-      <c r="M387" s="15"/>
-      <c r="N387" s="15"/>
-      <c r="O387" s="15"/>
-    </row>
-    <row r="388" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K388" s="15"/>
-      <c r="L388" s="15"/>
-      <c r="M388" s="15"/>
-      <c r="N388" s="15"/>
-      <c r="O388" s="15"/>
-    </row>
-    <row r="389" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K389" s="15"/>
-      <c r="L389" s="15"/>
-      <c r="M389" s="15"/>
-      <c r="N389" s="15"/>
-      <c r="O389" s="15"/>
-    </row>
-    <row r="390" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K390" s="15"/>
-      <c r="L390" s="15"/>
-      <c r="M390" s="15"/>
-      <c r="N390" s="15"/>
-      <c r="O390" s="15"/>
-    </row>
-    <row r="391" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K391" s="15"/>
-      <c r="L391" s="15"/>
-      <c r="M391" s="15"/>
-      <c r="N391" s="15"/>
-      <c r="O391" s="15"/>
-    </row>
-    <row r="392" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K392" s="15"/>
-      <c r="L392" s="15"/>
-      <c r="M392" s="15"/>
-      <c r="N392" s="15"/>
-      <c r="O392" s="15"/>
+      <c r="K385" s="10"/>
+      <c r="L385" s="10"/>
+      <c r="M385" s="10"/>
+      <c r="N385" s="10"/>
+      <c r="O385" s="10"/>
     </row>
     <row r="393" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K393" s="16"/>
-      <c r="L393" s="16"/>
-      <c r="M393" s="16"/>
-      <c r="N393" s="16"/>
-      <c r="O393" s="16"/>
-    </row>
-    <row r="394" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K394" s="15"/>
-      <c r="L394" s="15"/>
-      <c r="M394" s="15"/>
-      <c r="N394" s="15"/>
-      <c r="O394" s="15"/>
-    </row>
-    <row r="395" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K395" s="15"/>
-      <c r="L395" s="15"/>
-      <c r="M395" s="15"/>
-      <c r="N395" s="15"/>
-      <c r="O395" s="15"/>
-    </row>
-    <row r="396" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K396" s="15"/>
-      <c r="L396" s="15"/>
-      <c r="M396" s="15"/>
-      <c r="N396" s="15"/>
-      <c r="O396" s="15"/>
-    </row>
-    <row r="397" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K397" s="15"/>
-      <c r="L397" s="15"/>
-      <c r="M397" s="15"/>
-      <c r="N397" s="15"/>
-      <c r="O397" s="15"/>
-    </row>
-    <row r="398" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K398" s="15"/>
-      <c r="L398" s="15"/>
-      <c r="M398" s="15"/>
-      <c r="N398" s="15"/>
-      <c r="O398" s="15"/>
-    </row>
-    <row r="399" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K399" s="15"/>
-      <c r="L399" s="15"/>
-      <c r="M399" s="15"/>
-      <c r="N399" s="15"/>
-      <c r="O399" s="15"/>
-    </row>
-    <row r="400" spans="11:15" x14ac:dyDescent="0.15">
-      <c r="K400" s="15"/>
-      <c r="L400" s="15"/>
-      <c r="M400" s="15"/>
-      <c r="N400" s="15"/>
-      <c r="O400" s="15"/>
+      <c r="K393" s="10"/>
+      <c r="L393" s="10"/>
+      <c r="M393" s="10"/>
+      <c r="N393" s="10"/>
+      <c r="O393" s="10"/>
     </row>
     <row r="401" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B401" s="16"/>
-      <c r="C401" s="16"/>
-      <c r="D401" s="16"/>
-      <c r="E401" s="16"/>
-      <c r="F401" s="16"/>
-      <c r="K401" s="16"/>
-      <c r="L401" s="16"/>
-      <c r="M401" s="16"/>
-      <c r="N401" s="16"/>
-      <c r="O401" s="16"/>
-    </row>
-    <row r="402" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B402" s="15"/>
-      <c r="C402" s="15"/>
-      <c r="D402" s="15"/>
-      <c r="E402" s="15"/>
-      <c r="F402" s="15"/>
-      <c r="K402" s="15"/>
-      <c r="L402" s="15"/>
-      <c r="M402" s="15"/>
-      <c r="N402" s="15"/>
-      <c r="O402" s="15"/>
-    </row>
-    <row r="403" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B403" s="15"/>
-      <c r="C403" s="15"/>
-      <c r="D403" s="15"/>
-      <c r="E403" s="15"/>
-      <c r="F403" s="15"/>
-      <c r="K403" s="15"/>
-      <c r="L403" s="15"/>
-      <c r="M403" s="15"/>
-      <c r="N403" s="15"/>
-      <c r="O403" s="15"/>
-    </row>
-    <row r="404" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B404" s="15"/>
-      <c r="C404" s="15"/>
-      <c r="D404" s="15"/>
-      <c r="E404" s="15"/>
-      <c r="F404" s="15"/>
-      <c r="K404" s="15"/>
-      <c r="L404" s="15"/>
-      <c r="M404" s="15"/>
-      <c r="N404" s="15"/>
-      <c r="O404" s="15"/>
-    </row>
-    <row r="405" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B405" s="15"/>
-      <c r="C405" s="15"/>
-      <c r="D405" s="15"/>
-      <c r="E405" s="15"/>
-      <c r="F405" s="15"/>
-      <c r="K405" s="15"/>
-      <c r="L405" s="15"/>
-      <c r="M405" s="15"/>
-      <c r="N405" s="15"/>
-      <c r="O405" s="15"/>
-    </row>
-    <row r="406" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B406" s="15"/>
-      <c r="C406" s="15"/>
-      <c r="D406" s="15"/>
-      <c r="E406" s="15"/>
-      <c r="F406" s="15"/>
-      <c r="K406" s="15"/>
-      <c r="L406" s="15"/>
-      <c r="M406" s="15"/>
-      <c r="N406" s="15"/>
-      <c r="O406" s="15"/>
-    </row>
-    <row r="407" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B407" s="15"/>
-      <c r="C407" s="15"/>
-      <c r="D407" s="15"/>
-      <c r="E407" s="15"/>
-      <c r="F407" s="15"/>
+      <c r="B401" s="10"/>
+      <c r="C401" s="10"/>
+      <c r="D401" s="10"/>
+      <c r="E401" s="10"/>
+      <c r="F401" s="10"/>
+      <c r="K401" s="10"/>
+      <c r="L401" s="10"/>
+      <c r="M401" s="10"/>
+      <c r="N401" s="10"/>
+      <c r="O401" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="K71:O71"/>
+    <mergeCell ref="K61:O61"/>
+    <mergeCell ref="T25:X25"/>
     <mergeCell ref="K95:O95"/>
     <mergeCell ref="K108:O108"/>
     <mergeCell ref="K120:O120"/>
     <mergeCell ref="K130:O130"/>
     <mergeCell ref="K140:O140"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="K71:O71"/>
-    <mergeCell ref="K61:O61"/>
-    <mergeCell ref="T25:X25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>